<commit_message>
Print TMMC to console every BiasUpdate steps
</commit_message>
<xml_diff>
--- a/Confirmation_Results/Butane_TraPPE/Butane.xlsx
+++ b/Confirmation_Results/Butane_TraPPE/Butane.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett\Desktop\School\Thesis\TMMC\Confirmation_Results\Butane_TraPPE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7F53C0E-2047-4D30-BCEB-BF4780C83E73}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA931AF9-563F-4AD6-AC5F-79E021656308}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{F7692061-CD5F-4640-90A8-0918B792B80F}"/>
   </bookViews>
@@ -23550,16 +23550,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>61913</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>119062</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
-      <xdr:colOff>590551</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>152401</xdr:rowOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23887,7 +23887,7 @@
   <dimension ref="A1:N618"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24347,7 +24347,7 @@
         <v>532.0020012</v>
       </c>
       <c r="I13">
-        <f t="shared" ref="I13:I18" si="10">E13*$E$1</f>
+        <f t="shared" ref="I13:I17" si="10">E13*$E$1</f>
         <v>531.55157120000001</v>
       </c>
       <c r="J13" s="3">
@@ -24391,7 +24391,7 @@
         <v>545.3823875999999</v>
       </c>
       <c r="G14">
-        <f t="shared" ref="G13:G18" si="13">C14*$E$1</f>
+        <f t="shared" ref="G14:G18" si="13">C14*$E$1</f>
         <v>544.70064000000002</v>
       </c>
       <c r="H14">
@@ -24466,7 +24466,7 @@
         <v>564.26</v>
       </c>
       <c r="M15" s="7">
-        <f t="shared" ref="M14:M18" si="16">(J15-L15)/L15</f>
+        <f t="shared" ref="M15:M18" si="16">(J15-L15)/L15</f>
         <v>-1.1951759827029985E-2</v>
       </c>
       <c r="N15">
@@ -40806,11 +40806,11 @@
         <v>-20.902799999999999</v>
       </c>
       <c r="H543">
-        <f t="shared" ref="H543:H606" si="36">EXP(B543)*(A543+1)</f>
+        <f t="shared" ref="H543:H567" si="36">EXP(B543)*(A543+1)</f>
         <v>132995156.13100436</v>
       </c>
       <c r="I543">
-        <f t="shared" ref="I543:I606" si="37">EXP(B543)</f>
+        <f t="shared" ref="I543:I567" si="37">EXP(B543)</f>
         <v>258745.43994358825</v>
       </c>
     </row>

</xml_diff>